<commit_message>
Inputs ververst, Subjects-Classes allocations worden nu ook ingelezen. Kleine aanpassing Lesson Selection KB.
</commit_message>
<xml_diff>
--- a/inputs/klasseninfo.xlsx
+++ b/inputs/klasseninfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -504,7 +504,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -514,7 +514,7 @@
     <col min="3" max="4" width="6.5" customWidth="1"/>
     <col min="5" max="5" width="7.5" customWidth="1"/>
     <col min="6" max="6" width="8.1640625" customWidth="1"/>
-    <col min="7" max="7" width="50" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>